<commit_message>
ajout des projets + corrections ortho
</commit_message>
<xml_diff>
--- a/alves-de-paiva-julien-tableau-synthèse.xlsx
+++ b/alves-de-paiva-julien-tableau-synthèse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jalves\Documents\Julien - portfolio - oral 26-27.06.2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B4ACC4-EF7D-46D0-9DFF-F013F03E2821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FCA0E4-523D-4475-8A87-E1E9026A18B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E5" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>▢ SLAM</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio :</t>
-  </si>
-  <si>
     <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Simulation d'un parc de serveurs (sur le logiciel Vmware).</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://julienalvesdepaiva.github.io</t>
   </si>
 </sst>
 </file>
@@ -684,15 +684,39 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -724,30 +748,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1060,138 +1060,138 @@
   </sheetPr>
   <dimension ref="A1:AQ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B13"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="18.7109375" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="16384" width="10.85546875" style="1"/>
+    <col min="1" max="1" width="70.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="18.7265625" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.453125" customWidth="1"/>
+    <col min="44" max="16384" width="10.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="29"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="B6" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="H7" s="16" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1229,17 +1229,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1276,12 +1276,12 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="12"/>
@@ -1325,12 +1325,12 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -1374,12 +1374,12 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="17"/>
@@ -1423,7 +1423,7 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="8"/>
       <c r="C12" s="12"/>
@@ -1468,7 +1468,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="8"/>
       <c r="C13" s="12"/>
@@ -1513,17 +1513,17 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1560,12 +1560,12 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="12"/>
@@ -1609,12 +1609,12 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="12"/>
@@ -1658,12 +1658,12 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="17"/>
@@ -1707,12 +1707,12 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="17"/>
@@ -1756,12 +1756,12 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1805,7 +1805,7 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1850,65 +1850,65 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1919,17 +1919,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9afeb195-fe8e-4d53-b966-ac86e014f9d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b96438d6-4088-444b-a148-08e2a0c42289" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0540109B649AC4795630F51507852BE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b24b5783ddc2bb45fe34b7a1a06bc44d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9afeb195-fe8e-4d53-b966-ac86e014f9d0" xmlns:ns3="b96438d6-4088-444b-a148-08e2a0c42289" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="33a84ca242945553425b58f658027b0b" ns2:_="" ns3:_="">
     <xsd:import namespace="9afeb195-fe8e-4d53-b966-ac86e014f9d0"/>
@@ -2130,6 +2119,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9afeb195-fe8e-4d53-b966-ac86e014f9d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b96438d6-4088-444b-a148-08e2a0c42289" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2140,23 +2140,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA3166D-F719-49F0-B698-E9057D9EDF6C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b96438d6-4088-444b-a148-08e2a0c42289"/>
-    <ds:schemaRef ds:uri="9afeb195-fe8e-4d53-b966-ac86e014f9d0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65237427-9C7F-4709-8B62-3B4F8F99F7A0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2175,6 +2158,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EA3166D-F719-49F0-B698-E9057D9EDF6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b96438d6-4088-444b-a148-08e2a0c42289"/>
+    <ds:schemaRef ds:uri="9afeb195-fe8e-4d53-b966-ac86e014f9d0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{574C0259-CE3C-4D74-A0FE-24A73702E787}">
   <ds:schemaRefs>

</xml_diff>